<commit_message>
Update tree swallow R Project. Note: Data from 2017 and 2018 are not entered completely.
</commit_message>
<xml_diff>
--- a/data/2025_BET_nest_record_summary.xlsx
+++ b/data/2025_BET_nest_record_summary.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/randall_friendly_fws_gov1/Documents/Documents/Biological Programs/Tree Swallow Nest Box Monitoring/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfriendly\OneDrive - DOI\Documents\Biological Programs\Tree Swallow Nest Box Monitoring\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F5450D05-53CC-884D-9BA6-08404599A37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E18F4EF6-4234-48DA-A046-783882A766EC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032506D8-4CD5-460E-BB13-6AD0E30FA91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="4050" windowWidth="29040" windowHeight="15720" xr2:uid="{BD582D2F-836B-4721-9C05-C19BAEABB1A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="29">
   <si>
     <t>box_number</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>42B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -161,11 +167,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -502,36 +517,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1881F0DE-8046-47B1-8752-0A1E9DE2B4C9}">
-  <dimension ref="A1:X26"/>
+  <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="3" max="3" width="7.1796875" customWidth="1"/>
+    <col min="4" max="4" width="5.36328125" customWidth="1"/>
+    <col min="5" max="6" width="3.1796875" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" customWidth="1"/>
+    <col min="8" max="8" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.453125" customWidth="1"/>
     <col min="12" max="12" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="14.81640625" customWidth="1"/>
-    <col min="15" max="15" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1796875" style="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.36328125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.1796875" customWidth="1"/>
-    <col min="21" max="21" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.453125" customWidth="1"/>
-    <col min="23" max="23" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="17.1796875" style="3" customWidth="1"/>
+    <col min="21" max="21" width="18.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19" style="3" customWidth="1"/>
+    <col min="23" max="23" width="18.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -562,7 +576,7 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -577,7 +591,7 @@
       <c r="N1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -589,19 +603,19 @@
       <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="7" t="s">
         <v>16</v>
       </c>
       <c r="X1" s="1" t="s">
@@ -610,7 +624,7 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -622,27 +636,51 @@
         <v>2025</v>
       </c>
       <c r="G2" s="2">
-        <v>45804</v>
+        <v>45803</v>
       </c>
       <c r="H2" s="2">
-        <v>45810</v>
+        <v>45808</v>
       </c>
       <c r="I2" s="2">
-        <v>45809</v>
+        <v>45807</v>
       </c>
       <c r="J2" s="2">
-        <v>45823</v>
+        <v>45821</v>
       </c>
       <c r="K2" s="2">
-        <v>45824</v>
-      </c>
-      <c r="O2">
-        <v>7</v>
+        <v>45822</v>
+      </c>
+      <c r="L2" s="2">
+        <v>45838</v>
+      </c>
+      <c r="M2" s="2">
+        <v>45843</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="6">
+        <v>6</v>
+      </c>
+      <c r="P2">
+        <v>6</v>
+      </c>
+      <c r="Q2">
+        <v>6</v>
+      </c>
+      <c r="S2" s="8">
+        <v>45834</v>
+      </c>
+      <c r="T2" s="3">
+        <v>281100974</v>
+      </c>
+      <c r="W2" s="8">
+        <v>45833</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
@@ -654,27 +692,45 @@
         <v>2025</v>
       </c>
       <c r="G3" s="2">
-        <v>45803</v>
+        <v>45800</v>
       </c>
       <c r="H3" s="2">
-        <v>45808</v>
+        <v>45805</v>
       </c>
       <c r="I3" s="2">
-        <v>45807</v>
+        <v>45804</v>
       </c>
       <c r="J3" s="2">
-        <v>45821</v>
+        <v>45818</v>
       </c>
       <c r="K3" s="2">
         <v>45822</v>
       </c>
-      <c r="O3">
-        <v>6</v>
+      <c r="L3" s="2">
+        <v>45838</v>
+      </c>
+      <c r="M3" s="2">
+        <v>45840</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="6">
+        <v>6</v>
+      </c>
+      <c r="P3">
+        <v>6</v>
+      </c>
+      <c r="Q3">
+        <v>6</v>
+      </c>
+      <c r="W3" s="8">
+        <v>45834</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -686,19 +742,40 @@
         <v>2025</v>
       </c>
       <c r="G4" s="2">
-        <v>45804</v>
+        <v>45802</v>
       </c>
       <c r="H4" s="2">
-        <v>45809</v>
+        <v>45807</v>
       </c>
       <c r="I4" s="2">
-        <v>45808</v>
+        <v>45806</v>
       </c>
       <c r="J4" s="2">
+        <v>45820</v>
+      </c>
+      <c r="K4" s="2">
         <v>45822</v>
       </c>
-      <c r="O4">
-        <v>6</v>
+      <c r="L4" s="2">
+        <v>45838</v>
+      </c>
+      <c r="M4" s="2">
+        <v>45843</v>
+      </c>
+      <c r="N4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="6">
+        <v>6</v>
+      </c>
+      <c r="P4">
+        <v>6</v>
+      </c>
+      <c r="Q4">
+        <v>6</v>
+      </c>
+      <c r="W4" s="8">
+        <v>45833</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.35">
@@ -729,8 +806,38 @@
       <c r="K5" s="2">
         <v>45823</v>
       </c>
-      <c r="O5">
+      <c r="L5" s="2">
+        <v>45839</v>
+      </c>
+      <c r="M5" s="2">
+        <v>45843</v>
+      </c>
+      <c r="N5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="6">
         <v>7</v>
+      </c>
+      <c r="P5">
+        <v>6</v>
+      </c>
+      <c r="Q5">
+        <v>6</v>
+      </c>
+      <c r="S5" s="8">
+        <v>45834</v>
+      </c>
+      <c r="T5" s="3">
+        <v>160106636</v>
+      </c>
+      <c r="U5" s="8">
+        <v>45834</v>
+      </c>
+      <c r="V5" s="3">
+        <v>160106637</v>
+      </c>
+      <c r="W5" s="8">
+        <v>45834</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.35">
@@ -761,13 +868,43 @@
       <c r="K6" s="2">
         <v>45823</v>
       </c>
-      <c r="O6">
+      <c r="L6" s="2">
+        <v>45840</v>
+      </c>
+      <c r="M6" s="2">
+        <v>45843</v>
+      </c>
+      <c r="N6" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="6">
         <v>5</v>
+      </c>
+      <c r="P6">
+        <v>5</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="S6" s="8">
+        <v>45834</v>
+      </c>
+      <c r="T6" s="3">
+        <v>160106639</v>
+      </c>
+      <c r="U6" s="8">
+        <v>45834</v>
+      </c>
+      <c r="V6" s="3">
+        <v>160106638</v>
+      </c>
+      <c r="W6" s="8">
+        <v>45834</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
@@ -791,15 +928,34 @@
         <v>45821</v>
       </c>
       <c r="K7" s="2">
-        <v>45825</v>
-      </c>
-      <c r="O7">
-        <v>6</v>
+        <v>45823</v>
+      </c>
+      <c r="L7" s="2">
+        <v>45839</v>
+      </c>
+      <c r="M7" s="2">
+        <v>45843</v>
+      </c>
+      <c r="N7" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="6">
+        <v>6</v>
+      </c>
+      <c r="P7">
+        <v>6</v>
+      </c>
+      <c r="Q7">
+        <v>6</v>
+      </c>
+      <c r="U7" s="8"/>
+      <c r="W7" s="8">
+        <v>45835</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -823,15 +979,39 @@
         <v>45822</v>
       </c>
       <c r="K8" s="2">
-        <v>45825</v>
-      </c>
-      <c r="O8">
-        <v>6</v>
+        <v>45824</v>
+      </c>
+      <c r="L8" s="2">
+        <v>45840</v>
+      </c>
+      <c r="M8" s="2">
+        <v>45848</v>
+      </c>
+      <c r="N8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" s="6">
+        <v>6</v>
+      </c>
+      <c r="P8">
+        <v>6</v>
+      </c>
+      <c r="Q8">
+        <v>6</v>
+      </c>
+      <c r="U8" s="8">
+        <v>45835</v>
+      </c>
+      <c r="V8" s="3">
+        <v>160106660</v>
+      </c>
+      <c r="W8" s="8">
+        <v>45835</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>24</v>
@@ -857,13 +1037,31 @@
       <c r="K9" s="2">
         <v>45824</v>
       </c>
-      <c r="O9">
-        <v>6</v>
+      <c r="L9" s="2">
+        <v>45840</v>
+      </c>
+      <c r="M9" s="2">
+        <v>45843</v>
+      </c>
+      <c r="N9" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" s="6">
+        <v>6</v>
+      </c>
+      <c r="P9">
+        <v>6</v>
+      </c>
+      <c r="Q9">
+        <v>6</v>
+      </c>
+      <c r="W9" s="8">
+        <v>45833</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>24</v>
@@ -878,24 +1076,42 @@
         <v>45804</v>
       </c>
       <c r="H10" s="2">
+        <v>45810</v>
+      </c>
+      <c r="I10" s="2">
         <v>45809</v>
       </c>
-      <c r="I10" s="2">
-        <v>45808</v>
-      </c>
       <c r="J10" s="2">
-        <v>45822</v>
+        <v>45823</v>
       </c>
       <c r="K10" s="2">
-        <v>45825</v>
-      </c>
-      <c r="O10">
-        <v>6</v>
+        <v>45824</v>
+      </c>
+      <c r="L10" s="2">
+        <v>45840</v>
+      </c>
+      <c r="N10" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" s="6">
+        <v>7</v>
+      </c>
+      <c r="P10">
+        <v>7</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="U10" s="8">
+        <v>45835</v>
+      </c>
+      <c r="V10" s="3">
+        <v>160106645</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
@@ -907,27 +1123,57 @@
         <v>2025</v>
       </c>
       <c r="G11" s="2">
-        <v>45804</v>
+        <v>45803</v>
       </c>
       <c r="H11" s="2">
-        <v>45809</v>
+        <v>45808</v>
       </c>
       <c r="I11" s="2">
-        <v>45808</v>
+        <v>45807</v>
       </c>
       <c r="J11" s="2">
-        <v>45822</v>
+        <v>45821</v>
       </c>
       <c r="K11" s="2">
         <v>45825</v>
       </c>
-      <c r="O11">
-        <v>6</v>
+      <c r="L11" s="2">
+        <v>45841</v>
+      </c>
+      <c r="M11" s="2">
+        <v>45843</v>
+      </c>
+      <c r="N11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" s="6">
+        <v>6</v>
+      </c>
+      <c r="P11">
+        <v>6</v>
+      </c>
+      <c r="Q11">
+        <v>6</v>
+      </c>
+      <c r="S11" s="8">
+        <v>45834</v>
+      </c>
+      <c r="T11" s="3">
+        <v>160106725</v>
+      </c>
+      <c r="U11" s="8">
+        <v>45834</v>
+      </c>
+      <c r="V11" s="3">
+        <v>160106706</v>
+      </c>
+      <c r="W11" s="8">
+        <v>45836</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
         <v>24</v>
@@ -939,24 +1185,57 @@
         <v>2025</v>
       </c>
       <c r="G12" s="2">
-        <v>45800</v>
+        <v>45804</v>
       </c>
       <c r="H12" s="2">
-        <v>45804</v>
+        <v>45809</v>
       </c>
       <c r="I12" s="2">
-        <v>45805</v>
+        <v>45808</v>
       </c>
       <c r="J12" s="2">
-        <v>45819</v>
-      </c>
-      <c r="O12">
+        <v>45822</v>
+      </c>
+      <c r="K12" s="2">
+        <v>45825</v>
+      </c>
+      <c r="L12" s="2">
+        <v>45841</v>
+      </c>
+      <c r="M12" s="2">
+        <v>45848</v>
+      </c>
+      <c r="N12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O12" s="6">
+        <v>6</v>
+      </c>
+      <c r="P12">
         <v>5</v>
+      </c>
+      <c r="Q12">
+        <v>5</v>
+      </c>
+      <c r="S12" s="8">
+        <v>45834</v>
+      </c>
+      <c r="T12" s="3">
+        <v>160106635</v>
+      </c>
+      <c r="U12" s="8">
+        <v>45834</v>
+      </c>
+      <c r="V12" s="3">
+        <v>160106634</v>
+      </c>
+      <c r="W12" s="8">
+        <v>46201</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
@@ -968,27 +1247,51 @@
         <v>2025</v>
       </c>
       <c r="G13" s="2">
-        <v>45803</v>
+        <v>45804</v>
       </c>
       <c r="H13" s="2">
+        <v>45809</v>
+      </c>
+      <c r="I13" s="2">
         <v>45808</v>
       </c>
-      <c r="I13" s="2">
-        <v>45807</v>
-      </c>
       <c r="J13" s="2">
-        <v>45821</v>
+        <v>45822</v>
       </c>
       <c r="K13" s="2">
-        <v>45823</v>
-      </c>
-      <c r="O13">
-        <v>6</v>
+        <v>45825</v>
+      </c>
+      <c r="L13" s="2">
+        <v>45841</v>
+      </c>
+      <c r="M13" s="2">
+        <v>45848</v>
+      </c>
+      <c r="N13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" s="6">
+        <v>6</v>
+      </c>
+      <c r="P13">
+        <v>6</v>
+      </c>
+      <c r="Q13">
+        <v>6</v>
+      </c>
+      <c r="U13" s="8">
+        <v>45835</v>
+      </c>
+      <c r="V13" s="3">
+        <v>160106667</v>
+      </c>
+      <c r="W13" s="8">
+        <v>45835</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
@@ -1000,27 +1303,51 @@
         <v>2025</v>
       </c>
       <c r="G14" s="2">
-        <v>45802</v>
+        <v>45804</v>
       </c>
       <c r="H14" s="2">
-        <v>45807</v>
+        <v>45809</v>
       </c>
       <c r="I14" s="2">
-        <v>45806</v>
+        <v>45808</v>
       </c>
       <c r="J14" s="2">
-        <v>45820</v>
+        <v>45822</v>
       </c>
       <c r="K14" s="2">
-        <v>45822</v>
-      </c>
-      <c r="O14">
-        <v>6</v>
+        <v>45825</v>
+      </c>
+      <c r="L14" s="2">
+        <v>45841</v>
+      </c>
+      <c r="M14" s="2">
+        <v>45843</v>
+      </c>
+      <c r="N14" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" s="6">
+        <v>6</v>
+      </c>
+      <c r="P14">
+        <v>6</v>
+      </c>
+      <c r="Q14">
+        <v>6</v>
+      </c>
+      <c r="U14" s="8">
+        <v>45835</v>
+      </c>
+      <c r="V14" s="3">
+        <v>160106674</v>
+      </c>
+      <c r="W14" s="8">
+        <v>45835</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
         <v>24</v>
@@ -1044,15 +1371,45 @@
         <v>45822</v>
       </c>
       <c r="K15" s="2">
-        <v>45824</v>
-      </c>
-      <c r="O15">
-        <v>6</v>
+        <v>45825</v>
+      </c>
+      <c r="L15" s="2">
+        <v>45841</v>
+      </c>
+      <c r="M15" s="2">
+        <v>45851</v>
+      </c>
+      <c r="N15" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15" s="6">
+        <v>6</v>
+      </c>
+      <c r="P15">
+        <v>5</v>
+      </c>
+      <c r="Q15">
+        <v>4</v>
+      </c>
+      <c r="S15" s="8">
+        <v>45834</v>
+      </c>
+      <c r="T15" s="3">
+        <v>160106618</v>
+      </c>
+      <c r="U15" s="8">
+        <v>45834</v>
+      </c>
+      <c r="V15" s="3">
+        <v>160106619</v>
+      </c>
+      <c r="W15" s="8">
+        <v>45836</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>26</v>
+      <c r="A16">
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>24</v>
@@ -1064,24 +1421,48 @@
         <v>2025</v>
       </c>
       <c r="G16" s="2">
-        <v>45803</v>
+        <v>45805</v>
       </c>
       <c r="H16" s="2">
-        <v>45807</v>
+        <v>45809</v>
       </c>
       <c r="I16" s="2">
-        <v>45806</v>
+        <v>45808</v>
       </c>
       <c r="J16" s="2">
-        <v>45820</v>
-      </c>
-      <c r="O16">
+        <v>45822</v>
+      </c>
+      <c r="K16" s="2">
+        <v>45827</v>
+      </c>
+      <c r="L16" s="2">
+        <v>45843</v>
+      </c>
+      <c r="N16" t="s">
+        <v>27</v>
+      </c>
+      <c r="O16" s="6">
+        <v>6</v>
+      </c>
+      <c r="P16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="U16" s="8">
+        <v>45837</v>
+      </c>
+      <c r="V16" s="3">
+        <v>160106697</v>
+      </c>
+      <c r="W16" s="8">
+        <v>45837</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
         <v>24</v>
@@ -1104,13 +1485,40 @@
       <c r="J17" s="2">
         <v>45822</v>
       </c>
-      <c r="O17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="K17" s="2">
+        <v>45827</v>
+      </c>
+      <c r="L17" s="2">
+        <v>45843</v>
+      </c>
+      <c r="M17" s="2">
+        <v>45847</v>
+      </c>
+      <c r="N17" t="s">
+        <v>28</v>
+      </c>
+      <c r="O17" s="6">
+        <v>6</v>
+      </c>
+      <c r="P17">
+        <v>5</v>
+      </c>
+      <c r="Q17">
+        <v>5</v>
+      </c>
+      <c r="U17" s="8">
+        <v>45837</v>
+      </c>
+      <c r="V17" s="3">
+        <v>317184404</v>
+      </c>
+      <c r="W17" s="8">
+        <v>45837</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
         <v>24</v>
@@ -1122,248 +1530,536 @@
         <v>2025</v>
       </c>
       <c r="G18" s="2">
+        <v>45805</v>
+      </c>
+      <c r="H18" s="2">
+        <v>45810</v>
+      </c>
+      <c r="I18" s="2">
+        <v>45809</v>
+      </c>
+      <c r="J18" s="2">
+        <v>45823</v>
+      </c>
+      <c r="K18" s="2">
+        <v>45827</v>
+      </c>
+      <c r="L18" s="2">
+        <v>45843</v>
+      </c>
+      <c r="M18" s="2">
+        <v>45846</v>
+      </c>
+      <c r="N18" t="s">
+        <v>28</v>
+      </c>
+      <c r="O18" s="6">
+        <v>6</v>
+      </c>
+      <c r="P18">
+        <v>6</v>
+      </c>
+      <c r="Q18">
+        <v>6</v>
+      </c>
+      <c r="S18" s="8">
+        <v>45836</v>
+      </c>
+      <c r="T18" s="3">
+        <v>160106794</v>
+      </c>
+      <c r="U18" s="8">
+        <v>45836</v>
+      </c>
+      <c r="V18" s="3">
+        <v>160106747</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19">
+        <v>2025</v>
+      </c>
+      <c r="G19" s="2">
+        <v>45804</v>
+      </c>
+      <c r="H19" s="2">
+        <v>45809</v>
+      </c>
+      <c r="I19" s="2">
+        <v>45808</v>
+      </c>
+      <c r="J19" s="2">
+        <v>45822</v>
+      </c>
+      <c r="K19" s="2">
+        <v>45828</v>
+      </c>
+      <c r="L19" s="2">
+        <v>45844</v>
+      </c>
+      <c r="M19" s="2">
+        <v>45846</v>
+      </c>
+      <c r="N19" t="s">
+        <v>28</v>
+      </c>
+      <c r="O19" s="6">
+        <v>6</v>
+      </c>
+      <c r="P19">
+        <v>5</v>
+      </c>
+      <c r="Q19">
+        <v>5</v>
+      </c>
+      <c r="S19" s="8">
+        <v>45834</v>
+      </c>
+      <c r="T19" s="3">
+        <v>160106746</v>
+      </c>
+      <c r="U19" s="8">
+        <v>45834</v>
+      </c>
+      <c r="V19" s="3">
+        <v>160106627</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <v>2025</v>
+      </c>
+      <c r="G20" s="2">
+        <v>45804</v>
+      </c>
+      <c r="H20" s="2">
+        <v>45809</v>
+      </c>
+      <c r="I20" s="2">
+        <v>45808</v>
+      </c>
+      <c r="J20" s="2">
+        <v>45822</v>
+      </c>
+      <c r="K20" s="2">
+        <v>45828</v>
+      </c>
+      <c r="L20" s="2">
+        <v>45844</v>
+      </c>
+      <c r="M20" s="2">
+        <v>45847</v>
+      </c>
+      <c r="N20" t="s">
+        <v>28</v>
+      </c>
+      <c r="O20" s="6">
+        <v>6</v>
+      </c>
+      <c r="P20">
+        <v>5</v>
+      </c>
+      <c r="Q20">
+        <v>5</v>
+      </c>
+      <c r="W20" s="8">
+        <v>45837</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21">
+        <v>2025</v>
+      </c>
+      <c r="G21" s="2">
+        <v>45806</v>
+      </c>
+      <c r="H21" s="2">
+        <v>45810</v>
+      </c>
+      <c r="I21" s="2">
+        <v>45809</v>
+      </c>
+      <c r="J21" s="2">
+        <v>45823</v>
+      </c>
+      <c r="K21" s="2">
+        <v>45828</v>
+      </c>
+      <c r="L21" s="2">
+        <v>45844</v>
+      </c>
+      <c r="M21" s="2">
+        <v>45848</v>
+      </c>
+      <c r="N21" t="s">
+        <v>28</v>
+      </c>
+      <c r="O21" s="6">
+        <v>5</v>
+      </c>
+      <c r="P21">
+        <v>4</v>
+      </c>
+      <c r="Q21">
+        <v>4</v>
+      </c>
+      <c r="S21" s="8">
+        <v>45834</v>
+      </c>
+      <c r="T21" s="3">
+        <v>160106617</v>
+      </c>
+      <c r="U21" s="8">
+        <v>45834</v>
+      </c>
+      <c r="V21" s="3">
+        <v>160106616</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22">
+        <v>2025</v>
+      </c>
+      <c r="G22" s="2">
+        <v>45806</v>
+      </c>
+      <c r="H22" s="2">
+        <v>45812</v>
+      </c>
+      <c r="I22" s="2">
+        <v>45811</v>
+      </c>
+      <c r="J22" s="2">
+        <v>45825</v>
+      </c>
+      <c r="K22" s="2">
+        <v>45828</v>
+      </c>
+      <c r="L22" s="2">
+        <v>45844</v>
+      </c>
+      <c r="M22" s="2">
+        <v>45847</v>
+      </c>
+      <c r="N22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O22" s="6">
+        <v>7</v>
+      </c>
+      <c r="P22">
+        <v>6</v>
+      </c>
+      <c r="Q22">
+        <v>6</v>
+      </c>
+      <c r="S22" s="8">
+        <v>45835</v>
+      </c>
+      <c r="T22" s="3">
+        <v>160106797</v>
+      </c>
+      <c r="U22" s="8">
+        <v>45835</v>
+      </c>
+      <c r="V22" s="3">
+        <v>160106675</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23">
+        <v>2025</v>
+      </c>
+      <c r="G23" s="2">
+        <v>45808</v>
+      </c>
+      <c r="H23" s="2">
+        <v>45813</v>
+      </c>
+      <c r="I23" s="2">
+        <v>45812</v>
+      </c>
+      <c r="J23" s="2">
+        <v>45826</v>
+      </c>
+      <c r="K23" s="2">
+        <v>45828</v>
+      </c>
+      <c r="L23" s="2">
+        <v>45844</v>
+      </c>
+      <c r="M23" s="2">
+        <v>45851</v>
+      </c>
+      <c r="N23" t="s">
+        <v>28</v>
+      </c>
+      <c r="O23" s="6">
+        <v>6</v>
+      </c>
+      <c r="P23">
+        <v>6</v>
+      </c>
+      <c r="Q23">
+        <v>6</v>
+      </c>
+      <c r="S23" s="8">
+        <v>45836</v>
+      </c>
+      <c r="T23" s="3">
+        <v>160106693</v>
+      </c>
+      <c r="U23" s="8">
+        <v>45836</v>
+      </c>
+      <c r="V23" s="3">
+        <v>160106692</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24">
+        <v>2025</v>
+      </c>
+      <c r="G24" s="2">
+        <v>45811</v>
+      </c>
+      <c r="H24" s="2">
+        <v>45816</v>
+      </c>
+      <c r="I24" s="2">
+        <v>45815</v>
+      </c>
+      <c r="J24" s="2">
+        <v>45829</v>
+      </c>
+      <c r="K24" s="2">
+        <v>45830</v>
+      </c>
+      <c r="L24" s="2">
+        <v>45846</v>
+      </c>
+      <c r="M24" s="2">
+        <v>45851</v>
+      </c>
+      <c r="N24" t="s">
+        <v>28</v>
+      </c>
+      <c r="O24" s="6">
+        <v>6</v>
+      </c>
+      <c r="P24">
+        <v>6</v>
+      </c>
+      <c r="Q24">
+        <v>6</v>
+      </c>
+      <c r="S24" s="8">
+        <v>45837</v>
+      </c>
+      <c r="T24" s="3">
+        <v>317184409</v>
+      </c>
+      <c r="U24" s="8">
+        <v>45837</v>
+      </c>
+      <c r="V24" s="3">
+        <v>317184410</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25">
+        <v>2025</v>
+      </c>
+      <c r="G25" s="2">
+        <v>45813</v>
+      </c>
+      <c r="H25" s="2">
+        <v>45816</v>
+      </c>
+      <c r="I25" s="2">
+        <v>45815</v>
+      </c>
+      <c r="J25" s="2">
+        <v>45829</v>
+      </c>
+      <c r="K25" s="2">
+        <v>45831</v>
+      </c>
+      <c r="L25" s="2">
+        <v>45847</v>
+      </c>
+      <c r="M25" s="2">
+        <v>45853</v>
+      </c>
+      <c r="N25" t="s">
+        <v>28</v>
+      </c>
+      <c r="O25" s="6">
+        <v>4</v>
+      </c>
+      <c r="P25">
+        <v>4</v>
+      </c>
+      <c r="Q25">
+        <v>4</v>
+      </c>
+      <c r="S25" s="8">
+        <v>45835</v>
+      </c>
+      <c r="T25" s="3">
+        <v>160106647</v>
+      </c>
+      <c r="U25" s="8">
+        <v>45835</v>
+      </c>
+      <c r="V25" s="3">
+        <v>160106646</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <v>2025</v>
+      </c>
+      <c r="G26" s="2">
         <v>45800</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H26" s="2">
+        <v>45804</v>
+      </c>
+      <c r="I26" s="2">
         <v>45805</v>
       </c>
-      <c r="I18" s="2">
-        <v>45804</v>
-      </c>
-      <c r="J18" s="2">
-        <v>45818</v>
-      </c>
-      <c r="K18" s="2">
-        <v>45822</v>
-      </c>
-      <c r="O18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19">
-        <v>2025</v>
-      </c>
-      <c r="G19" s="2">
+      <c r="J26" s="2">
+        <v>45819</v>
+      </c>
+      <c r="N26" t="s">
+        <v>27</v>
+      </c>
+      <c r="O26" s="6">
+        <v>5</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27">
+        <v>2025</v>
+      </c>
+      <c r="G27" s="2">
+        <v>45803</v>
+      </c>
+      <c r="H27" s="2">
+        <v>45807</v>
+      </c>
+      <c r="I27" s="2">
         <v>45806</v>
       </c>
-      <c r="H19" s="2">
-        <v>45810</v>
-      </c>
-      <c r="I19" s="2">
-        <v>45809</v>
-      </c>
-      <c r="J19" s="2">
-        <v>45823</v>
-      </c>
-      <c r="O19">
+      <c r="J27" s="2">
+        <v>45820</v>
+      </c>
+      <c r="N27" t="s">
+        <v>27</v>
+      </c>
+      <c r="O27" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20">
-        <v>2025</v>
-      </c>
-      <c r="G20" s="2">
-        <v>45806</v>
-      </c>
-      <c r="H20" s="2">
-        <v>45812</v>
-      </c>
-      <c r="I20" s="2">
-        <v>45811</v>
-      </c>
-      <c r="J20" s="2">
-        <v>45825</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21">
-        <v>2025</v>
-      </c>
-      <c r="G21" s="2">
-        <v>45805</v>
-      </c>
-      <c r="H21" s="2">
-        <v>45809</v>
-      </c>
-      <c r="I21" s="2">
-        <v>45808</v>
-      </c>
-      <c r="J21" s="2">
-        <v>45822</v>
-      </c>
-      <c r="O21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>44</v>
-      </c>
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22">
-        <v>2025</v>
-      </c>
-      <c r="G22" s="2">
-        <v>45804</v>
-      </c>
-      <c r="H22" s="2">
-        <v>45809</v>
-      </c>
-      <c r="I22" s="2">
-        <v>45808</v>
-      </c>
-      <c r="J22" s="2">
-        <v>45822</v>
-      </c>
-      <c r="O22">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>13</v>
-      </c>
-      <c r="B23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23">
-        <v>2025</v>
-      </c>
-      <c r="G23" s="2">
-        <v>45804</v>
-      </c>
-      <c r="H23" s="2">
-        <v>45809</v>
-      </c>
-      <c r="I23" s="2">
-        <v>45808</v>
-      </c>
-      <c r="J23" s="2">
-        <v>45822</v>
-      </c>
-      <c r="O23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>41</v>
-      </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24">
-        <v>2025</v>
-      </c>
-      <c r="G24" s="2">
-        <v>45808</v>
-      </c>
-      <c r="H24" s="2">
-        <v>45813</v>
-      </c>
-      <c r="I24" s="2">
-        <v>45812</v>
-      </c>
-      <c r="J24" s="2">
-        <v>45826</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>40</v>
-      </c>
-      <c r="B25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25">
-        <v>2025</v>
-      </c>
-      <c r="G25" s="2">
-        <v>45805</v>
-      </c>
-      <c r="H25" s="2">
-        <v>45810</v>
-      </c>
-      <c r="I25" s="2">
-        <v>45809</v>
-      </c>
-      <c r="J25" s="2">
-        <v>45823</v>
-      </c>
-      <c r="O25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>30</v>
-      </c>
-      <c r="B26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26">
-        <v>2025</v>
-      </c>
-      <c r="G26" s="2">
-        <v>45811</v>
-      </c>
-      <c r="H26" s="2">
-        <v>45816</v>
-      </c>
-      <c r="I26" s="2">
-        <v>45815</v>
-      </c>
-      <c r="J26" s="2">
-        <v>45829</v>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X27">
+    <sortCondition ref="K1:K27"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>